<commit_message>
Update actividades bggws 2018.xlsx
cambio en el archivo excel
</commit_message>
<xml_diff>
--- a/actividades bggws 2018.xlsx
+++ b/actividades bggws 2018.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CesarBernaola\Desktop\PRUEBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA97243-34E2-41C7-82FB-FE61D6202E2B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>PERÚ</t>
   </si>
@@ -76,12 +82,15 @@
   </si>
   <si>
     <t>Validación e inventario de reportes diarios de las rutinas batch de Perú y Bolivia</t>
+  </si>
+  <si>
+    <t>Actividad de prueba excel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,7 +435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -562,11 +571,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B4:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +625,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>